<commit_message>
April 3 - Maya
Airplane data spreadsheet is complete with 10 planes added.

Plane class works well and aisles are implemented to be the correct width in different sections of the plane.
</commit_message>
<xml_diff>
--- a/airplane data.xlsx
+++ b/airplane data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28724"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/mshapi01_uoguelph_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2289941-54EC-4D93-953F-107F0CB1DFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="8_{1AFD09AA-24B5-4129-B4A8-0A8B97C2209F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79C3D8AD-C1D5-4B54-80E0-ACEDB926CD8A}"/>
   <bookViews>
-    <workbookView xWindow="1866" yWindow="1716" windowWidth="17280" windowHeight="9984" xr2:uid="{39F7129E-1D30-432A-A69C-DA8458EF82C5}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{39F7129E-1D30-432A-A69C-DA8458EF82C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>aircraft_type</t>
   </si>
@@ -44,7 +44,7 @@
     <t>airline</t>
   </si>
   <si>
-    <t>total seats</t>
+    <t>total seats - economy</t>
   </si>
   <si>
     <t>seat width - economy</t>
@@ -65,6 +65,9 @@
     <t>seat arrangement - business</t>
   </si>
   <si>
+    <t>total seats - business</t>
+  </si>
+  <si>
     <t>seat width - first class</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
     <t>seat arrangement - first class</t>
   </si>
   <si>
+    <t>total seats - first class</t>
+  </si>
+  <si>
     <t>A220-300</t>
   </si>
   <si>
@@ -92,20 +98,62 @@
     <t>1 2</t>
   </si>
   <si>
-    <t>total seats - first class</t>
-  </si>
-  <si>
-    <t>total seats - business</t>
-  </si>
-  <si>
-    <t>total seats - economy</t>
+    <t>Beechcraft 1900D</t>
+  </si>
+  <si>
+    <t>1 1</t>
+  </si>
+  <si>
+    <t>Boeing 737-300 (733)</t>
+  </si>
+  <si>
+    <t>Lion Airlines</t>
+  </si>
+  <si>
+    <t>3 3</t>
+  </si>
+  <si>
+    <t>Airbus A319 (319) Layout 1</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>Embraer E-175 (E75) Layout 1</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Airbus A320-200 (320)</t>
+  </si>
+  <si>
+    <t>Condor</t>
+  </si>
+  <si>
+    <t>Boeing 737-700 Layout 2</t>
+  </si>
+  <si>
+    <t>SpiceJet</t>
+  </si>
+  <si>
+    <t>ATR 72-600 (ATR)</t>
+  </si>
+  <si>
+    <t>Air France</t>
+  </si>
+  <si>
+    <t>Boeing 717-200 (717)</t>
+  </si>
+  <si>
+    <t>Hawaiian Airlines</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,31 +522,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4DF597-2E11-4719-8A39-DDAC5DB33C10}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="23.68359375" customWidth="1"/>
-    <col min="4" max="4" width="18.578125" customWidth="1"/>
-    <col min="5" max="5" width="25.578125" customWidth="1"/>
-    <col min="6" max="6" width="28.15625" customWidth="1"/>
-    <col min="7" max="7" width="19.15625" customWidth="1"/>
-    <col min="8" max="8" width="18.578125" customWidth="1"/>
-    <col min="9" max="9" width="25.578125" customWidth="1"/>
-    <col min="10" max="10" width="28.15625" customWidth="1"/>
-    <col min="11" max="11" width="19.15625" customWidth="1"/>
-    <col min="12" max="12" width="18.578125" customWidth="1"/>
-    <col min="13" max="13" width="25.578125" customWidth="1"/>
-    <col min="14" max="14" width="28.15625" customWidth="1"/>
-    <col min="15" max="15" width="19.15625" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" ht="29.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +567,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -530,27 +579,27 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>137</v>
@@ -562,7 +611,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>125</v>
@@ -574,7 +623,7 @@
         <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K2">
         <v>12</v>
@@ -583,12 +632,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" ht="15">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>76</v>
@@ -600,7 +649,7 @@
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>64</v>
@@ -612,13 +661,305 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K3">
         <v>12</v>
       </c>
       <c r="O3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>20.2</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>18</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>150</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>128</v>
+      </c>
+      <c r="D6">
+        <v>17.7</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6">
+        <v>78</v>
+      </c>
+      <c r="H6">
+        <v>17.7</v>
+      </c>
+      <c r="I6">
+        <v>34</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>42</v>
+      </c>
+      <c r="L6">
+        <v>20.5</v>
+      </c>
+      <c r="M6">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7">
+        <v>76</v>
+      </c>
+      <c r="D7">
+        <v>18.25</v>
+      </c>
+      <c r="E7">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>52</v>
+      </c>
+      <c r="H7">
+        <v>18.25</v>
+      </c>
+      <c r="I7">
+        <v>34</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7">
+        <v>37</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>164</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>132</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <v>32</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9">
+        <v>134</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>126</v>
+      </c>
+      <c r="H9">
+        <v>19</v>
+      </c>
+      <c r="I9">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>72</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>31</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10">
+        <v>72</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11">
+        <v>128</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>120</v>
+      </c>
+      <c r="L11">
+        <v>18.5</v>
+      </c>
+      <c r="M11">
+        <v>37</v>
+      </c>
+      <c r="N11" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -636,6 +977,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072AAD56A75A2D94FB3A091E80440349E" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f226472916d10b344db84c18f6d4c359">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d8ee30fa-356b-4bb2-891a-28d344d6702f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="494c5678af19c6158bb8ae1fbe9e3424" ns2:_="">
     <xsd:import namespace="d8ee30fa-356b-4bb2-891a-28d344d6702f"/>
@@ -773,45 +1120,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EEE4CD2-9540-46C6-9425-F3CC01F93F68}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EEE4CD2-9540-46C6-9425-F3CC01F93F68}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD407948-1DF5-428D-9A2B-FBDF3FA575E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d8ee30fa-356b-4bb2-891a-28d344d6702f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AFA1948-74DF-4088-A071-D74146EEAB26}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AFA1948-74DF-4088-A071-D74146EEAB26}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD407948-1DF5-428D-9A2B-FBDF3FA575E0}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>